<commit_message>
update final exam time
</commit_message>
<xml_diff>
--- a/LectureSpring2019.xlsx
+++ b/LectureSpring2019.xlsx
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="143">
   <si>
     <t>Week</t>
   </si>
@@ -495,6 +495,12 @@
   </si>
   <si>
     <t>[Power and Effect-size](https://crumplab.github.io/psyc3400/Presentations/6d_power.html#1)</t>
+  </si>
+  <si>
+    <t>M May 20</t>
+  </si>
+  <si>
+    <t>M May 20 10:30AM - 12:30 PM</t>
   </si>
 </sst>
 </file>
@@ -835,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1406,10 +1412,10 @@
         <v>79</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>133</v>
@@ -1461,6 +1467,12 @@
       <c r="F49"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>141</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="D50" s="1" t="s">
         <v>51</v>
       </c>

</xml_diff>